<commit_message>
renamed:    Trading/TR_USAA/HAA_TR.json -> Trading/TR_USAA/USAA_TR.json 	modified:   Trading/TR_USAA/USAA_Trading.py 	renamed:    Trading/TR_USAA/HAA_data.json -> Trading/TR_USAA/USAA_data.json 	modified:   "\354\265\234\354\242\205_\354\227\260\352\270\210_\354\213\234\353\256\254\353\240\210\354\235\264\354\205\230_\354\225\204\355\214\214\355\212\270\353\263\264\354\234\240.xlsx"
</commit_message>
<xml_diff>
--- a/최종_연금_시뮬레이션_아파트보유.xlsx
+++ b/최종_연금_시뮬레이션_아파트보유.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ilpus\Desktop\git_folder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E753BE38-6345-413E-876F-A25C87019E7B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEFD5F43-101E-4399-9770-D6E88FC9EBE5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2039,8 +2039,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E80" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I102" sqref="I102"/>
+    <sheetView tabSelected="1" topLeftCell="B44" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O90" sqref="O90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="16.5"/>
@@ -2564,7 +2564,7 @@
         <v>124</v>
       </c>
       <c r="B42" s="29">
-        <v>0.2</v>
+        <v>0.15</v>
       </c>
       <c r="C42" s="38" t="s">
         <v>127</v>
@@ -4451,11 +4451,11 @@
       </c>
       <c r="C84" s="54">
         <f>D84+E84+F84+G84</f>
-        <v>1016647898.74</v>
+        <v>995809831.69000006</v>
       </c>
       <c r="D84" s="43">
         <f>416761341*(1+B$42)-3000000</f>
-        <v>497113609.19999999</v>
+        <v>476275542.14999998</v>
       </c>
       <c r="E84" s="54">
         <f>316008759*(1+B$43)</f>
@@ -4504,7 +4504,7 @@
       </c>
       <c r="X84" s="34">
         <f>W84+V84+U84+K84+J84+I84+H84+C84</f>
-        <v>2023372073.0550001</v>
+        <v>2002534006.0050001</v>
       </c>
       <c r="Y84" s="68" t="s">
         <v>137</v>
@@ -4523,11 +4523,11 @@
       </c>
       <c r="C85" s="54">
         <f>D85+E85+F85+G85</f>
-        <v>1094956935.9004002</v>
+        <v>1046137478.3329</v>
       </c>
       <c r="D85" s="85">
         <f>D84*(1+B$42)-29000000-20000000</f>
-        <v>547536331.03999996</v>
+        <v>498716873.47249997</v>
       </c>
       <c r="E85" s="86">
         <f>E84*(1+B$43)-10000000</f>
@@ -4579,7 +4579,7 @@
       </c>
       <c r="X85" s="34">
         <f>W85+V85+U85+K85+J85+I85+H85+C85+T85</f>
-        <v>2198060181.5458751</v>
+        <v>2149240723.978375</v>
       </c>
       <c r="Y85" s="68" t="s">
         <v>145</v>
@@ -4597,11 +4597,11 @@
       </c>
       <c r="C86" s="54">
         <f t="shared" ref="C86:C87" si="10">D86+E86+F86+G86</f>
-        <v>1236696923.7182162</v>
+        <v>1153177730.9635911</v>
       </c>
       <c r="D86" s="43">
         <f t="shared" ref="D86" si="11">D85*(1+B$42)-29000000</f>
-        <v>628043597.24799991</v>
+        <v>544524404.49337494</v>
       </c>
       <c r="E86" s="54">
         <f t="shared" ref="E86:E88" si="12">E85*(1+B$43)</f>
@@ -4654,7 +4654,7 @@
       </c>
       <c r="X86" s="34">
         <f t="shared" ref="X86:X87" si="15">W86+V86+U86+K86+J86+I86+H86+C86+T86</f>
-        <v>2404065880.330647</v>
+        <v>2320546687.5760221</v>
       </c>
       <c r="Y86" s="68" t="s">
         <v>138</v>
@@ -4672,11 +4672,11 @@
       </c>
       <c r="C87" s="73">
         <f t="shared" si="10"/>
-        <v>1371490010.9383476</v>
+        <v>1244040759.4081287</v>
       </c>
       <c r="D87" s="74">
         <f>D86*(1+B$42)-29000000-30000000</f>
-        <v>694652316.69759989</v>
+        <v>567203065.16738117</v>
       </c>
       <c r="E87" s="73">
         <f>E86*(1+B$43)</f>
@@ -4729,7 +4729,7 @@
       </c>
       <c r="X87" s="78">
         <f t="shared" si="15"/>
-        <v>2641601249.7305861</v>
+        <v>2514151998.2003675</v>
       </c>
       <c r="Y87" s="68" t="s">
         <v>140</v>
@@ -4745,11 +4745,11 @@
       </c>
       <c r="C88" s="54">
         <f>D88+E88+F88+G88</f>
-        <v>1577355017.2783444</v>
+        <v>1396055762.1837127</v>
       </c>
       <c r="D88" s="43">
         <f>D87*(1+B$42)-9000000</f>
-        <v>824582780.03711987</v>
+        <v>643283524.94248831</v>
       </c>
       <c r="E88" s="54">
         <f t="shared" si="12"/>
@@ -4803,7 +4803,7 @@
       </c>
       <c r="X88" s="34">
         <f>W88+V88+U88+K88+J88+I88+H88+C88</f>
-        <v>2846126113.5920787</v>
+        <v>2664826858.497447</v>
       </c>
       <c r="Y88" s="70" t="s">
         <v>139</v>
@@ -4818,23 +4818,23 @@
         <v>58</v>
       </c>
       <c r="C89" s="60">
-        <f t="shared" ref="C89:C90" si="16">D89+E89+F89+G89</f>
-        <v>1786847393.9925778</v>
+        <f>D89+E89+F89+G89</f>
+        <v>1537124111.6318955</v>
       </c>
       <c r="D89" s="74">
         <f>D88*(1+B$42)-40000000</f>
-        <v>949499336.04454374</v>
+        <v>699776053.68386149</v>
       </c>
       <c r="E89" s="60">
         <f>E88*(1+B$43)</f>
         <v>608010063.63104391</v>
       </c>
       <c r="F89" s="60">
-        <f t="shared" ref="F89" si="17">F88*(1+D$42)</f>
+        <f t="shared" ref="F89" si="16">F88*(1+D$42)</f>
         <v>84171181.436263099</v>
       </c>
       <c r="G89" s="47">
-        <f t="shared" ref="G89" si="18">G88*(1+D$43)</f>
+        <f t="shared" ref="G89" si="17">G88*(1+D$43)</f>
         <v>145166812.88072708</v>
       </c>
       <c r="H89" s="47">
@@ -4877,7 +4877,7 @@
       </c>
       <c r="X89" s="79">
         <f>W89+V89+U89+K89+J89+I89+H89+C89</f>
-        <v>3082683199.1667051</v>
+        <v>2832959916.8060226</v>
       </c>
       <c r="Z89" s="20">
         <f>Z82+SUM(Z83:Z88)</f>
@@ -4892,12 +4892,12 @@
         <v>59</v>
       </c>
       <c r="C90" s="80">
-        <f t="shared" si="16"/>
-        <v>2070958844.6401858</v>
+        <f t="shared" ref="C89:C90" si="18">D90+E90+F90+G90</f>
+        <v>1736302103.1231742</v>
       </c>
       <c r="D90" s="81">
         <f>D89*(1+B$42)</f>
-        <v>1139399203.2534525</v>
+        <v>804742461.73644066</v>
       </c>
       <c r="E90" s="80">
         <f>E89*(1+B$43)</f>
@@ -4969,11 +4969,11 @@
       </c>
       <c r="C91" s="80">
         <f t="shared" ref="C91:C92" si="23">D91+E91+F91+G91</f>
-        <v>2203795977.3358617</v>
+        <v>1761970764.4286253</v>
       </c>
       <c r="D91" s="89">
         <f>D90*(1+B$42)-200000000</f>
-        <v>1167279043.9041431</v>
+        <v>725453830.99690664</v>
       </c>
       <c r="E91" s="80">
         <f>E90*(1+B$43)</f>
@@ -5048,11 +5048,11 @@
       </c>
       <c r="C92" s="80">
         <f t="shared" si="23"/>
-        <v>2554193690.6156926</v>
+        <v>1987730743.5771639</v>
       </c>
       <c r="D92" s="81">
         <f t="shared" ref="D92:D114" si="32">D91*(1+B$42)</f>
-        <v>1400734852.6849716</v>
+        <v>834271905.64644253</v>
       </c>
       <c r="E92" s="80">
         <f t="shared" ref="E92:E114" si="33">E91*(1+B$43)</f>
@@ -5124,11 +5124,11 @@
       </c>
       <c r="C93" s="80">
         <f t="shared" ref="C93:C114" si="36">D93+E93+F93+G93</f>
-        <v>2964650123.2531114</v>
+        <v>2243180991.5245543</v>
       </c>
       <c r="D93" s="81">
         <f t="shared" si="32"/>
-        <v>1680881823.2219658</v>
+        <v>959412691.4934088</v>
       </c>
       <c r="E93" s="80">
         <f t="shared" si="33"/>
@@ -5183,7 +5183,7 @@
         <v>96.82175013402572</v>
       </c>
       <c r="S93" s="34">
-        <f t="shared" si="31"/>
+        <f>S92+P93</f>
         <v>119618516.91398701</v>
       </c>
       <c r="T93" s="43">
@@ -5200,11 +5200,11 @@
       </c>
       <c r="C94" s="80">
         <f t="shared" si="36"/>
-        <v>3446047350.762701</v>
+        <v>2532313758.1137624</v>
       </c>
       <c r="D94" s="81">
         <f t="shared" si="32"/>
-        <v>2017058187.8663588</v>
+        <v>1103324595.2174201</v>
       </c>
       <c r="E94" s="80">
         <f t="shared" si="33"/>
@@ -5277,11 +5277,11 @@
       </c>
       <c r="C95" s="80">
         <f t="shared" si="36"/>
-        <v>4011314832.601614</v>
+        <v>2859668291.6620159</v>
       </c>
       <c r="D95" s="81">
         <f t="shared" si="32"/>
-        <v>2420469825.4396305</v>
+        <v>1268823284.5000329</v>
       </c>
       <c r="E95" s="80">
         <f t="shared" si="33"/>
@@ -5354,11 +5354,11 @@
       </c>
       <c r="C96" s="80">
         <f t="shared" si="36"/>
-        <v>4575823997.8029795</v>
+        <v>3130406984.4504609</v>
       </c>
       <c r="D96" s="89">
         <f>D95*(1+B$42)-100000000</f>
-        <v>2804563790.5275564</v>
+        <v>1359146777.1750376</v>
       </c>
       <c r="E96" s="80">
         <f t="shared" si="33"/>
@@ -5437,11 +5437,11 @@
       </c>
       <c r="C97" s="80">
         <f t="shared" si="36"/>
-        <v>5337860015.2301865</v>
+        <v>3535402260.3484116</v>
       </c>
       <c r="D97" s="81">
         <f t="shared" si="32"/>
-        <v>3365476548.6330676</v>
+        <v>1563018793.7512932</v>
       </c>
       <c r="E97" s="80">
         <f t="shared" si="33"/>
@@ -5514,11 +5514,11 @@
       </c>
       <c r="C98" s="80">
         <f t="shared" si="36"/>
-        <v>6235185982.5327435</v>
+        <v>3994085736.9870501</v>
       </c>
       <c r="D98" s="81">
         <f t="shared" si="32"/>
-        <v>4038571858.3596811</v>
+        <v>1797471612.813987</v>
       </c>
       <c r="E98" s="80">
         <f t="shared" si="33"/>
@@ -5591,11 +5591,11 @@
       </c>
       <c r="C99" s="80">
         <f t="shared" si="36"/>
-        <v>7292917790.8342113</v>
+        <v>4513723915.5386791</v>
       </c>
       <c r="D99" s="81">
         <f t="shared" si="32"/>
-        <v>4846286230.0316172</v>
+        <v>2067092354.7360849</v>
       </c>
       <c r="E99" s="80">
         <f t="shared" si="33"/>
@@ -5672,11 +5672,11 @@
       </c>
       <c r="C100" s="80">
         <f t="shared" si="36"/>
-        <v>8540971546.9034138</v>
+        <v>5102584278.8119717</v>
       </c>
       <c r="D100" s="81">
         <f t="shared" si="32"/>
-        <v>5815543476.03794</v>
+        <v>2377156207.9464974</v>
       </c>
       <c r="E100" s="80">
         <f t="shared" si="33"/>
@@ -5753,11 +5753,11 @@
       </c>
       <c r="C101" s="80">
         <f t="shared" si="36"/>
-        <v>9014997781.0722065</v>
+        <v>4770075248.9651499</v>
       </c>
       <c r="D101" s="89">
         <f>D100*(1+B$42)-1000000000</f>
-        <v>5978652171.2455282</v>
+        <v>1733729639.1384721</v>
       </c>
       <c r="E101" s="80">
         <f t="shared" si="33"/>
@@ -5833,11 +5833,11 @@
       </c>
       <c r="C102" s="80">
         <f t="shared" si="36"/>
-        <v>10557499481.450846</v>
+        <v>5376905960.965456</v>
       </c>
       <c r="D102" s="81">
         <f t="shared" si="32"/>
-        <v>7174382605.4946337</v>
+        <v>1993789085.0092428</v>
       </c>
       <c r="E102" s="80">
         <f t="shared" si="33"/>
@@ -5914,11 +5914,11 @@
       </c>
       <c r="C103" s="80">
         <f t="shared" si="36"/>
-        <v>12379170365.792919</v>
+        <v>6062768686.9599876</v>
       </c>
       <c r="D103" s="81">
         <f t="shared" si="32"/>
-        <v>8609259126.5935593</v>
+        <v>2292857447.7606292</v>
       </c>
       <c r="E103" s="80">
         <f t="shared" si="33"/>
@@ -5995,11 +5995,11 @@
       </c>
       <c r="C104" s="80">
         <f t="shared" si="36"/>
-        <v>14532497042.910469</v>
+        <v>6838172155.9229183</v>
       </c>
       <c r="D104" s="81">
         <f t="shared" si="32"/>
-        <v>10331110951.912271</v>
+        <v>2636786064.9247231</v>
       </c>
       <c r="E104" s="80">
         <f t="shared" si="33"/>
@@ -6072,11 +6072,11 @@
       </c>
       <c r="C105" s="80">
         <f t="shared" si="36"/>
-        <v>17080077399.263079</v>
+        <v>7715048231.6317854</v>
       </c>
       <c r="D105" s="81">
         <f t="shared" si="32"/>
-        <v>12397333142.294725</v>
+        <v>3032303974.6634312</v>
       </c>
       <c r="E105" s="80">
         <f t="shared" si="33"/>
@@ -6149,11 +6149,11 @@
       </c>
       <c r="C106" s="80">
         <f t="shared" si="36"/>
-        <v>20096597961.291286</v>
+        <v>8706947761.4005585</v>
       </c>
       <c r="D106" s="81">
         <f t="shared" si="32"/>
-        <v>14876799770.75367</v>
+        <v>3487149570.8629456</v>
       </c>
       <c r="E106" s="80">
         <f t="shared" si="33"/>
@@ -6226,11 +6226,11 @@
       </c>
       <c r="C107" s="80">
         <f t="shared" si="36"/>
-        <v>23671201475.824757</v>
+        <v>9829263757.412735</v>
       </c>
       <c r="D107" s="81">
         <f t="shared" si="32"/>
-        <v>17852159724.904404</v>
+        <v>4010222006.4923873</v>
       </c>
       <c r="E107" s="80">
         <f t="shared" si="33"/>
@@ -6303,11 +6303,11 @@
       </c>
       <c r="C108" s="80">
         <f t="shared" si="36"/>
-        <v>27910322134.098927</v>
+        <v>11099485771.679884</v>
       </c>
       <c r="D108" s="81">
         <f t="shared" si="32"/>
-        <v>21422591669.885284</v>
+        <v>4611755307.4662447</v>
       </c>
       <c r="E108" s="80">
         <f t="shared" si="33"/>
@@ -6380,11 +6380,11 @@
       </c>
       <c r="C109" s="80">
         <f t="shared" si="36"/>
-        <v>32941081277.02858</v>
+        <v>12537489876.752426</v>
       </c>
       <c r="D109" s="81">
         <f t="shared" si="32"/>
-        <v>25707110003.862339</v>
+        <v>5303518603.5861807</v>
       </c>
       <c r="E109" s="80">
         <f t="shared" si="33"/>
@@ -6457,11 +6457,11 @@
       </c>
       <c r="C110" s="80">
         <f t="shared" si="36"/>
-        <v>38915354905.278152</v>
+        <v>14165869294.76746</v>
       </c>
       <c r="D110" s="81">
         <f t="shared" si="32"/>
-        <v>30848532004.634808</v>
+        <v>6099046394.1241074</v>
       </c>
       <c r="E110" s="80">
         <f t="shared" si="33"/>
@@ -6534,11 +6534,11 @@
       </c>
       <c r="C111" s="80">
         <f t="shared" si="36"/>
-        <v>46014646491.064735</v>
+        <v>16010311438.745691</v>
       </c>
       <c r="D111" s="81">
         <f t="shared" si="32"/>
-        <v>37018238405.561768</v>
+        <v>7013903353.2427225</v>
       </c>
       <c r="E111" s="80">
         <f t="shared" si="33"/>
@@ -6611,11 +6611,11 @@
       </c>
       <c r="C112" s="80">
         <f t="shared" si="36"/>
-        <v>54455925185.882881</v>
+        <v>18100027955.437889</v>
       </c>
       <c r="D112" s="81">
         <f t="shared" si="32"/>
-        <v>44421886086.674118</v>
+        <v>8065988856.2291298</v>
       </c>
       <c r="E112" s="80">
         <f t="shared" si="33"/>
@@ -6688,11 +6688,11 @@
       </c>
       <c r="C113" s="80">
         <f t="shared" si="36"/>
-        <v>64498621422.936295</v>
+        <v>20468245303.590851</v>
       </c>
       <c r="D113" s="81">
         <f t="shared" si="32"/>
-        <v>53306263304.008942</v>
+        <v>9275887184.6634979</v>
       </c>
       <c r="E113" s="80">
         <f t="shared" si="33"/>
@@ -6765,11 +6765,11 @@
       </c>
       <c r="C114" s="80">
         <f t="shared" si="36"/>
-        <v>76453010185.029694</v>
+        <v>23152764482.581997</v>
       </c>
       <c r="D114" s="81">
         <f t="shared" si="32"/>
-        <v>63967515964.81073</v>
+        <v>10667270262.363022</v>
       </c>
       <c r="E114" s="80">
         <f t="shared" si="33"/>

</xml_diff>